<commit_message>
Tidsregistering og genoprettelse af fil Laura fik slettet
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/DT Tidstagning.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/DT Tidstagning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danat\Google Drev\Skole\Datamatiker\Eclipse\Workspaces\PTE-projekt\Documentation\08 - Project Management\Tidsregistrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danat\git\PTE-projekt\Documentation\08 - Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -123,15 +123,6 @@
     <t>Stakeholder</t>
   </si>
   <si>
-    <t>Navn:</t>
-  </si>
-  <si>
-    <t>Rolle:</t>
-  </si>
-  <si>
-    <t>Dato:</t>
-  </si>
-  <si>
     <t>Ulla Larsen</t>
   </si>
   <si>
@@ -180,27 +171,9 @@
     <t>Dan A. Toft</t>
   </si>
   <si>
-    <t>Aktivitet:</t>
-  </si>
-  <si>
-    <t>Starttid:</t>
-  </si>
-  <si>
-    <t>Sluttid:</t>
-  </si>
-  <si>
-    <t>Samlet tid brugt (timer):</t>
-  </si>
-  <si>
     <t>* Hvis du er i tvivl om din rolle, så kig i Appendiks A i "Rational Unified Process" (PDF side: 304 - 310) Bogen side 273 - 280)</t>
   </si>
   <si>
-    <t>TIDSREGISTRERING FOR PTE-PROJEKTET (6-3-2017  -  24-3-2017)</t>
-  </si>
-  <si>
-    <t>DT</t>
-  </si>
-  <si>
     <t>GITHUB</t>
   </si>
   <si>
@@ -214,6 +187,42 @@
   </si>
   <si>
     <t>Brugertest</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>TIDSREGISTRERING FOR PTE-PROJEKTET</t>
+  </si>
+  <si>
+    <t>Sluttid</t>
+  </si>
+  <si>
+    <t>Starttid</t>
+  </si>
+  <si>
+    <t>Aktivitet</t>
+  </si>
+  <si>
+    <t>Rolle</t>
+  </si>
+  <si>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>UC1: SSD</t>
+  </si>
+  <si>
+    <t>UC 1,2: SSD REVIEW</t>
+  </si>
+  <si>
+    <t>GITHUB ala Flemming</t>
+  </si>
+  <si>
+    <t>Post-it opsætter</t>
+  </si>
+  <si>
+    <t>Review af OC1</t>
   </si>
 </sst>
 </file>
@@ -221,10 +230,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="hh:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +249,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -257,11 +273,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -277,13 +393,196 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="hh:mm;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="hh:mm;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -294,6 +593,98 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>132769</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1334661" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rektangel 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48161FB-F116-467C-BF57-B581F8502442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1942519" y="0"/>
+          <a:ext cx="1334661" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="da-DK" sz="5400" b="1" cap="none" spc="0">
+              <a:ln/>
+              <a:pattFill prst="dkUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Dan</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="B5:G45" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B5:G45"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Dato" dataDxfId="5"/>
+    <tableColumn id="2" name="Rolle" dataDxfId="4"/>
+    <tableColumn id="3" name="Aktivitet" dataDxfId="3"/>
+    <tableColumn id="4" name="Starttid" dataDxfId="2">
+      <calculatedColumnFormula>IF(B6=B5,F5,TIME(8,5,0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Sluttid" dataDxfId="1"/>
+    <tableColumn id="6" name="Timer" dataDxfId="0">
+      <calculatedColumnFormula>(F6-E6)*24</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,296 +984,910 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+    <row r="2" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="B3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>42800</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" ref="E6:E45" si="0">IF(B6=B5,F5,TIME(8,5,0))</f>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="G6" s="12">
+        <f>(F6-E6)*24</f>
+        <v>7.416666666666667</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <f t="shared" ref="B7:B45" si="1">IF(F6&gt;=TIME(15,30,0),B6+1,B6)</f>
+        <v>42801</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="G7" s="12">
+        <f>(F7-E7)*24</f>
+        <v>2.4166666666666661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <f t="shared" si="1"/>
+        <v>42801</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.4375</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" ref="G8:G17" si="2">(F8-E8)*24</f>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <f t="shared" si="1"/>
+        <v>42801</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42800</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
         <v>0.33680555555555558</v>
       </c>
-      <c r="F4" s="8">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="G4">
-        <f>(F4-E4)*24</f>
-        <v>7.416666666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42801</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.33680555555555558</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.4375</v>
-      </c>
-      <c r="G5">
-        <f>(F5-E5)*24</f>
-        <v>2.4166666666666661</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42801</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.4375</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ref="G6:G15" si="0">(F6-E6)*24</f>
+      <c r="F10" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666607</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="2"/>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="2"/>
         <v>1.0000000000000004</v>
       </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>42801</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B13" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="2"/>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B14" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.49999999999999822</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B15" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="12">
+        <f t="shared" si="2"/>
+        <v>-14.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="G18" s="7"/>
+      <c r="B18" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="12">
+        <f t="shared" ref="G18:G34" si="3">(F18-E18)*24</f>
+        <v>0</v>
+      </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="G19" s="7"/>
+      <c r="B19" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="G20" s="7"/>
+      <c r="B20" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="G21" s="7"/>
+      <c r="B21" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="G22" s="7"/>
+      <c r="B22" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="7"/>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="7"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H24" s="7"/>
     </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="12">
+        <f t="shared" ref="G35:G45" si="4">(F35-E35)*24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="16"/>
+      <c r="E42" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="11">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16:E102">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E46:E113">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions headings="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -899,7 +1904,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -922,82 +1927,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>